<commit_message>
feat(catalogue): add table.mappedTo refback
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CatalogueCentralDictionaries.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CatalogueCentralDictionaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDEAECD-4DCD-9247-B759-1A507F8B4A71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B34D32B-073C-494E-A4D1-4C9F8C5EF2A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13423" uniqueCount="3651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13428" uniqueCount="3652">
   <si>
     <t>name</t>
   </si>
@@ -11056,6 +11056,9 @@
   </si>
   <si>
     <t>ontologyTermIRI</t>
+  </si>
+  <si>
+    <t>mappingsTo</t>
   </si>
 </sst>
 </file>
@@ -11530,13 +11533,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11743,47 +11746,37 @@
         <v>3605</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>3651</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>3604</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>3619</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
         <v>3601</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L12" s="20" t="s">
         <v>3610</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>3601</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>3598</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="I12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>3634</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>3606</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>3601</v>
       </c>
-      <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>609</v>
+        <v>3598</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>19</v>
@@ -11792,19 +11785,16 @@
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>3598</v>
-      </c>
-      <c r="H13" s="5"/>
+        <v>621</v>
+      </c>
       <c r="I13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>3634</v>
+      </c>
       <c r="L13" s="5" t="s">
-        <v>618</v>
+        <v>3606</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -11813,16 +11803,20 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>0</v>
+        <v>609</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>3598</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="b">
         <v>1</v>
@@ -11830,7 +11824,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -11839,85 +11833,89 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5" t="s">
-        <v>3597</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>3601</v>
       </c>
+      <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>3597</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>3601</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>3603</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>3611</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>3625</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>3612</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+    <row r="18" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B18" s="20" t="s">
         <v>3601</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20" t="s">
         <v>3614</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -11925,13 +11923,15 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -11945,23 +11945,19 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -11969,14 +11965,14 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -11984,7 +11980,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -11993,21 +11989,23 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="L22" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
@@ -12015,25 +12013,21 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>613</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
+        <v>169</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>3598</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -12041,20 +12035,24 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>10</v>
+        <v>613</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>3598</v>
+      </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -12063,10 +12061,10 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>10</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -12075,7 +12073,9 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="L25" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -12083,10 +12083,10 @@
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -12095,44 +12095,40 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="5" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
-        <v>3649</v>
+        <v>24</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
-        <v>3648</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
-        <v>594</v>
-      </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
@@ -12140,17 +12136,19 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
-        <v>616</v>
+        <v>3649</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
-        <v>617</v>
+        <v>3648</v>
       </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>594</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -12162,103 +12160,102 @@
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>3602</v>
+        <v>617</v>
       </c>
       <c r="G30" s="5"/>
-      <c r="H30" s="5" t="s">
-        <v>3638</v>
-      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
-      <c r="L30" s="5" t="s">
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>3602</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>3638</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5" t="s">
         <v>3615</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="21" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
+    <row r="32" spans="1:12" s="21" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="20" t="s">
         <v>3602</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B32" s="20" t="s">
         <v>3601</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20" t="s">
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20" t="s">
         <v>3613</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
         <v>3602</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5" t="s">
         <v>3638</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5" t="s">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>3598</v>
       </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5" t="b">
+      <c r="H33" s="5"/>
+      <c r="I33" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5" t="s">
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5" t="s">
         <v>3616</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
+    <row r="34" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
         <v>3648</v>
       </c>
-      <c r="L33" s="20" t="s">
+      <c r="L34" s="20" t="s">
         <v>3617</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
-        <v>3648</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>3598</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="5">
-        <v>1</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="I34" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>3634</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12266,7 +12263,7 @@
         <v>3648</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>594</v>
+        <v>3598</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>19</v>
@@ -12275,16 +12272,13 @@
         <v>1</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>3598</v>
+        <v>621</v>
       </c>
       <c r="I35" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="L35" s="5" t="s">
-        <v>36</v>
+      <c r="J35" s="5" t="s">
+        <v>3634</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12292,19 +12286,25 @@
         <v>3648</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>86</v>
+        <v>594</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
       </c>
+      <c r="F36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>3598</v>
+      </c>
       <c r="I36" s="5" t="b">
         <v>1</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12312,13 +12312,19 @@
         <v>3648</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="E37" s="5">
+        <v>1</v>
+      </c>
       <c r="I37" s="5" t="b">
         <v>1</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12326,10 +12332,13 @@
         <v>3648</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="I38" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12337,10 +12346,10 @@
         <v>3648</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>593</v>
+        <v>87</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12348,41 +12357,32 @@
         <v>3648</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
+        <v>3648</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>3650</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>3618</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="20" t="s">
+    <row r="42" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="20" t="s">
         <v>3611</v>
       </c>
-      <c r="L41" s="20" t="s">
+      <c r="L42" s="20" t="s">
         <v>3621</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>3611</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>3622</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" s="5">
-        <v>1</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="I42" s="5" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12390,7 +12390,7 @@
         <v>3611</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>3619</v>
+        <v>3622</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>19</v>
@@ -12399,10 +12399,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>3622</v>
+        <v>621</v>
       </c>
       <c r="I43" s="5" t="b">
         <v>1</v>
@@ -12413,19 +12410,22 @@
         <v>3611</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="E44" s="5">
+        <v>1</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>3601</v>
+        <v>608</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>3619</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>3623</v>
+        <v>3622</v>
+      </c>
+      <c r="I44" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12433,19 +12433,19 @@
         <v>3611</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>3624</v>
+        <v>3620</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="5">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="I45" s="5" t="b">
-        <v>1</v>
+        <v>3601</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>3619</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>3623</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12453,7 +12453,7 @@
         <v>3611</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>3628</v>
+        <v>3624</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>19</v>
@@ -12462,10 +12462,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>3624</v>
+        <v>621</v>
       </c>
       <c r="I46" s="5" t="b">
         <v>1</v>
@@ -12476,7 +12473,7 @@
         <v>3611</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>3625</v>
+        <v>3628</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>19</v>
@@ -12485,16 +12482,13 @@
         <v>1</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>3601</v>
+        <v>608</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>3628</v>
+        <v>3624</v>
       </c>
       <c r="I47" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12502,19 +12496,25 @@
         <v>3611</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>39</v>
+        <v>3625</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="E48" s="5">
+        <v>1</v>
+      </c>
       <c r="F48" s="5" t="s">
-        <v>32</v>
+        <v>3601</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>3628</v>
       </c>
       <c r="I48" s="5" t="b">
         <v>1</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>40</v>
+        <v>474</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12522,16 +12522,19 @@
         <v>3611</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="I49" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12539,13 +12542,16 @@
         <v>3611</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>3626</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12553,13 +12559,13 @@
         <v>3611</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>450</v>
+        <v>2</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>7</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>453</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12567,73 +12573,61 @@
         <v>3611</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>43</v>
+        <v>450</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>7</v>
       </c>
       <c r="L52" s="5" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>3611</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L53" s="5" t="s">
         <v>3633</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="20" t="s">
+    <row r="54" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="20" t="s">
         <v>3604</v>
       </c>
-      <c r="L53" s="20" t="s">
+      <c r="L54" s="20" t="s">
         <v>3627</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
-        <v>3604</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>3622</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" s="20">
-        <v>1</v>
-      </c>
-      <c r="F54" s="22" t="s">
-        <v>621</v>
-      </c>
-      <c r="I54" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="22" t="s">
-        <v>3631</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>3604</v>
       </c>
+      <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
-        <v>3619</v>
-      </c>
-      <c r="D55" s="5" t="s">
+        <v>3622</v>
+      </c>
+      <c r="D55" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="20">
         <v>1</v>
       </c>
-      <c r="F55" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>3622</v>
-      </c>
-      <c r="I55" s="5" t="b">
+      <c r="F55" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="I55" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="L55" s="5" t="s">
-        <v>3629</v>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22" t="s">
+        <v>3631</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12641,7 +12635,7 @@
         <v>3604</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>3624</v>
+        <v>3619</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>19</v>
@@ -12650,13 +12644,16 @@
         <v>1</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>621</v>
+        <v>608</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>3622</v>
       </c>
       <c r="I56" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="L56" s="22" t="s">
-        <v>3632</v>
+      <c r="L56" s="5" t="s">
+        <v>3629</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12664,7 +12661,7 @@
         <v>3604</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>3628</v>
+        <v>3624</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>19</v>
@@ -12673,16 +12670,13 @@
         <v>1</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>3624</v>
+        <v>621</v>
       </c>
       <c r="I57" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="L57" s="5" t="s">
-        <v>3630</v>
+      <c r="L57" s="22" t="s">
+        <v>3632</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12690,13 +12684,25 @@
         <v>3604</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>87</v>
+        <v>3628</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="E58" s="5">
+        <v>1</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>3624</v>
+      </c>
+      <c r="I58" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>572</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -12704,39 +12710,53 @@
         <v>3604</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>3626</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>3604</v>
       </c>
-      <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
       <c r="L60" s="5" t="s">
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>3604</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5" t="s">
         <v>3633</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M40" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:M41" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>